<commit_message>
SE3: Written the Abstract and Intro, AA1: Updated the logbook, KU7: Updated the Project
</commit_message>
<xml_diff>
--- a/Doc/Project Plan_weekly.xlsx
+++ b/Doc/Project Plan_weekly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcastedu.sharepoint.com/sites/msteams_564c74/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C515258-4805-4C30-BD3C-625EB5CF95BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{064E48CC-FF20-47D7-A2F0-248D409EC418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5490" yWindow="4758" windowWidth="21600" windowHeight="11010" activeTab="1" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
+    <workbookView minimized="1" xWindow="5490" yWindow="4758" windowWidth="21600" windowHeight="11010" firstSheet="1" activeTab="1" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
   </bookViews>
   <sheets>
     <sheet name="Projected" sheetId="1" r:id="rId1"/>
@@ -245,7 +245,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +299,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFBFBFBF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -731,7 +738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -796,6 +803,7 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2145,7 +2153,7 @@
   <dimension ref="B1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2434,8 +2442,8 @@
       <c r="I12" s="51"/>
       <c r="J12" s="51"/>
       <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
       <c r="N12" s="32"/>
       <c r="O12" s="32"/>
       <c r="P12" s="32"/>
@@ -2607,7 +2615,7 @@
       <c r="Q20" s="37"/>
       <c r="R20" s="38"/>
     </row>
-    <row r="21" spans="2:18">
+    <row r="21" spans="2:18" ht="15">
       <c r="B21" s="11"/>
       <c r="C21" s="1" t="s">
         <v>47</v>
@@ -2620,7 +2628,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
+      <c r="L21" s="62"/>
       <c r="M21" s="32"/>
       <c r="N21" s="32"/>
       <c r="O21" s="32"/>
@@ -2628,7 +2636,7 @@
       <c r="Q21" s="37"/>
       <c r="R21" s="38"/>
     </row>
-    <row r="22" spans="2:18">
+    <row r="22" spans="2:18" ht="15">
       <c r="B22" s="11"/>
       <c r="C22" s="1" t="s">
         <v>48</v>
@@ -2641,7 +2649,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
+      <c r="L22" s="62"/>
       <c r="M22" s="32"/>
       <c r="N22" s="32"/>
       <c r="O22" s="32"/>
@@ -3117,7 +3125,7 @@
       <c r="J45" s="32"/>
       <c r="K45" s="32"/>
       <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
+      <c r="M45" s="14"/>
       <c r="N45" s="32"/>
       <c r="O45" s="32"/>
       <c r="P45" s="32"/>
@@ -3137,7 +3145,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="32"/>
       <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
+      <c r="L46" s="14"/>
       <c r="M46" s="32"/>
       <c r="N46" s="32"/>
       <c r="O46" s="32"/>
@@ -3172,21 +3180,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100504F0EFF1BE61D46A34440DDC749B165" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6861fccdae819c068e3d2675729df3bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29ddf0ed-477c-451e-8755-cfaffaaa5733" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6fc745dc185d8196f008ac861e10f643" ns2:_="">
     <xsd:import namespace="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
@@ -3318,8 +3311,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD7FEF4-E84B-468B-9D19-73896C646B9B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3327,5 +3335,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD7FEF4-E84B-468B-9D19-73896C646B9B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}"/>
 </file>
</xml_diff>